<commit_message>
Work in progress Jan 16 / Excel with variables
</commit_message>
<xml_diff>
--- a/grafana/home/centos/EnvVariables.xlsx
+++ b/grafana/home/centos/EnvVariables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sg0549743/_github/influxdata/grafana/home/centos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFCCCDFC-800C-3D41-B731-AD73AB722DF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185C1639-71EA-0D42-957F-EB983840A21D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="1480" windowWidth="28040" windowHeight="17440" xr2:uid="{1061F871-5F9A-3646-AB6A-760BDF813E99}"/>
+    <workbookView xWindow="-31100" yWindow="720" windowWidth="41000" windowHeight="17440" xr2:uid="{1061F871-5F9A-3646-AB6A-760BDF813E99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -124,6 +124,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,14 +154,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,149 +494,155 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="49.1640625" customWidth="1"/>
-    <col min="3" max="3" width="59" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="75.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>8086</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="11" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{9A2B1AB0-A39C-C848-9530-53D7FD926083}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{0EC30B5D-A3B5-F047-841A-8DD9D3990D75}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{75D36983-20E1-0A47-88BB-9DB3619FB0E8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>